<commit_message>
Add 90I back to the enum and code tables.
</commit_message>
<xml_diff>
--- a/tools/nibrs-staging-data/src/test/resources/codeSpreadSheets/NIBRSCodeTablesGeneral.xlsx
+++ b/tools/nibrs-staging-data/src/test/resources/codeSpreadSheets/NIBRSCodeTablesGeneral.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="24300" yWindow="3240" windowWidth="20240" windowHeight="12180" tabRatio="705" firstSheet="28" activeTab="30"/>
+    <workbookView xWindow="480" yWindow="480" windowWidth="25120" windowHeight="15040" tabRatio="705" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2240" uniqueCount="693">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2248" uniqueCount="695">
   <si>
     <t>Table</t>
   </si>
@@ -2129,6 +2129,12 @@
   </si>
   <si>
     <t>Not a Cargo Theft offense</t>
+  </si>
+  <si>
+    <t>90I</t>
+  </si>
+  <si>
+    <t>Runaway</t>
   </si>
 </sst>
 </file>
@@ -2188,9 +2194,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="120">
+  <cellStyleXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2328,7 +2336,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="120">
+  <cellStyles count="122">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -2388,6 +2396,7 @@
     <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -2447,6 +2456,7 @@
     <cellStyle name="Hyperlink" xfId="114" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="118" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="120" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="TableStyleLight1" xfId="1"/>
   </cellStyles>
@@ -9396,7 +9406,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -9621,10 +9631,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I66"/>
+  <dimension ref="A1:I67"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:I28"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58:E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -11296,19 +11306,19 @@
     </row>
     <row r="58" spans="1:9" ht="15" customHeight="1">
       <c r="A58" s="1">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>632</v>
+        <v>693</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>633</v>
+        <v>694</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>632</v>
+        <v>693</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>633</v>
+        <v>694</v>
       </c>
       <c r="F58" s="1" t="s">
         <v>615</v>
@@ -11325,19 +11335,19 @@
     </row>
     <row r="59" spans="1:9" ht="15" customHeight="1">
       <c r="A59" s="1">
-        <v>990</v>
+        <v>910</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>615</v>
@@ -11346,27 +11356,27 @@
         <v>169</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>636</v>
+        <v>619</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>169</v>
+        <v>584</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="15" customHeight="1">
       <c r="A60" s="1">
-        <v>701</v>
-      </c>
-      <c r="B60" s="7">
-        <v>720</v>
+        <v>990</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>634</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>637</v>
-      </c>
-      <c r="D60" s="7">
-        <v>720</v>
+        <v>635</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>634</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="F60" s="1" t="s">
         <v>615</v>
@@ -11375,27 +11385,27 @@
         <v>169</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>619</v>
+        <v>636</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" ht="15" customHeight="1">
       <c r="A61" s="1">
-        <v>702</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>638</v>
+        <v>701</v>
+      </c>
+      <c r="B61" s="7">
+        <v>720</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>639</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>638</v>
+        <v>637</v>
+      </c>
+      <c r="D61" s="7">
+        <v>720</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="F61" s="1" t="s">
         <v>615</v>
@@ -11404,27 +11414,27 @@
         <v>169</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>640</v>
+        <v>619</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>528</v>
+        <v>584</v>
       </c>
     </row>
     <row r="62" spans="1:9">
       <c r="A62" s="1">
-        <v>403</v>
+        <v>702</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="F62" s="1" t="s">
         <v>615</v>
@@ -11433,56 +11443,56 @@
         <v>169</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>584</v>
+        <v>528</v>
       </c>
     </row>
     <row r="63" spans="1:9">
       <c r="A63" s="1">
+        <v>403</v>
+      </c>
+      <c r="B63" s="2" t="s">
         <v>641</v>
       </c>
-      <c r="B63" s="2" t="s">
-        <v>644</v>
-      </c>
       <c r="C63" s="1" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>526</v>
+        <v>615</v>
       </c>
       <c r="G63" s="1" t="s">
         <v>169</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>528</v>
+        <v>584</v>
       </c>
     </row>
     <row r="64" spans="1:9">
       <c r="A64" s="1">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>526</v>
@@ -11499,59 +11509,88 @@
     </row>
     <row r="65" spans="1:9">
       <c r="A65" s="1">
-        <v>99999</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>649</v>
+        <v>642</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>647</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>649</v>
+        <v>648</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>647</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>170</v>
+        <v>648</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>170</v>
+        <v>526</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>170</v>
+        <v>646</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>170</v>
+        <v>528</v>
       </c>
     </row>
     <row r="66" spans="1:9">
       <c r="A66" s="1">
+        <v>99999</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>649</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>649</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="I66" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
+      <c r="A67" s="1">
         <v>99998</v>
       </c>
-      <c r="B66" s="3" t="s">
+      <c r="B67" s="3" t="s">
         <v>505</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="C67" s="1" t="s">
         <v>506</v>
       </c>
-      <c r="D66" s="3" t="s">
+      <c r="D67" s="3" t="s">
         <v>505</v>
       </c>
-      <c r="E66" s="1" t="s">
+      <c r="E67" s="1" t="s">
         <v>506</v>
       </c>
-      <c r="F66" s="1" t="s">
+      <c r="F67" s="1" t="s">
         <v>506</v>
       </c>
-      <c r="G66" s="1" t="s">
+      <c r="G67" s="1" t="s">
         <v>506</v>
       </c>
-      <c r="H66" s="1" t="s">
+      <c r="H67" s="1" t="s">
         <v>506</v>
       </c>
-      <c r="I66" s="1" t="s">
+      <c r="I67" s="1" t="s">
         <v>506</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add R Replace code to the SegmentActionTypeType code table.
</commit_message>
<xml_diff>
--- a/tools/nibrs-staging-data/src/test/resources/codeSpreadSheets/NIBRSCodeTablesGeneral.xlsx
+++ b/tools/nibrs-staging-data/src/test/resources/codeSpreadSheets/NIBRSCodeTablesGeneral.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="480" windowWidth="25120" windowHeight="15040" tabRatio="705" activeTab="3"/>
+    <workbookView xWindow="22640" yWindow="1440" windowWidth="25120" windowHeight="15040" tabRatio="705" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2248" uniqueCount="695">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2252" uniqueCount="696">
   <si>
     <t>Table</t>
   </si>
@@ -2135,6 +2135,9 @@
   </si>
   <si>
     <t>Runaway</t>
+  </si>
+  <si>
+    <t>Replace</t>
   </si>
 </sst>
 </file>
@@ -6814,10 +6817,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6894,37 +6897,54 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5">
-        <v>99999</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="C5" t="s">
-        <v>170</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>383</v>
+    <row r="5" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>695</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>246</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>170</v>
+        <v>695</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6">
+        <v>99999</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>383</v>
+      </c>
+      <c r="C6" t="s">
+        <v>170</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>383</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7">
         <v>99998</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>505</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>506</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>505</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>506</v>
       </c>
     </row>
@@ -9633,7 +9653,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+    <sheetView topLeftCell="A48" workbookViewId="0">
       <selection activeCell="D58" sqref="D58:E58"/>
     </sheetView>
   </sheetViews>

</xml_diff>